<commit_message>
Add new sheet to test files
</commit_message>
<xml_diff>
--- a/workspace/tests/files/invalid_excel_configuration.xlsx
+++ b/workspace/tests/files/invalid_excel_configuration.xlsx
@@ -10,6 +10,7 @@
     <sheet name="TAB-A" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="TAB-B" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Extra" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ExposureGroup &lt;-&gt; Portname" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -642,4 +643,119 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ExposureGroup</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Portname</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>USHU_Hurricane_Full</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>USHU</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>USEQ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>USEQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>USFL_Flood_Full</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>USFL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CBHU_Hurricane_Full</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CBHU</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CBEQ_QuakeBC</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CBEQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MEHU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MEHU</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PRHU</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PRHU</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>